<commit_message>
finished readme, fixed name in cmake
</commit_message>
<xml_diff>
--- a/gemm/mklblas/benchmarks/chart.xlsx
+++ b/gemm/mklblas/benchmarks/chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\prace\CodeVault\hpc_kernel_samples\dense_linear_algebra\gemm\gemm_tbb_lapac\benchmarks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\prace\CodeVault\hpc_kernel_samples\dense_linear_algebra\gemm\mklblas\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -133,7 +133,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-AT" baseline="0"/>
-              <a:t> Multiplication Benchmark</a:t>
+              <a:t>-Matrix Multiplication Benchmark</a:t>
             </a:r>
             <a:endParaRPr lang="de-AT"/>
           </a:p>
@@ -180,7 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$12</c:f>
+              <c:f>Tabelle1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -215,7 +215,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$13:$C$23</c:f>
+              <c:f>Tabelle1!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -257,42 +257,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$13:$D$23</c:f>
+              <c:f>Tabelle1!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.5166300000000001E-8</c:v>
+                  <c:v>2.8573699999999999E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2736299999999994E-8</c:v>
+                  <c:v>8.40742E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1895199999999998E-7</c:v>
+                  <c:v>2.4041000000000002E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.15487E-6</c:v>
+                  <c:v>1.2213399999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1165299999999997E-6</c:v>
+                  <c:v>5.8142000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.68291E-5</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>2.2247200000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>1.5610699999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>1.42416E-2</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>0.111112</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>1.66299</c:v>
+                  <c:v>3.7852499999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2039E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8858499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5963999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11711000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8560300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,7 +309,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$E$12</c:f>
+              <c:f>Tabelle1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -344,7 +344,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$13:$C$23</c:f>
+              <c:f>Tabelle1!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -386,42 +386,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$13:$E$23</c:f>
+              <c:f>Tabelle1!$E$3:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.7379200000000001E-8</c:v>
+                  <c:v>3.4290999999999999E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1905299999999997E-8</c:v>
+                  <c:v>8.1853499999999999E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8974899999999998E-7</c:v>
+                  <c:v>3.8938699999999999E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8606199999999999E-6</c:v>
+                  <c:v>2.8687000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7921900000000001E-5</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>2.6095900000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>2.3298799999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>1.9121099999999999E-2</c:v>
+                  <c:v>2.7430700000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6868999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.55719E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.10762E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25542700000000002</c:v>
+                  <c:v>0.29692600000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7526299999999999</c:v>
+                  <c:v>3.0330599999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>65.6952</c:v>
+                  <c:v>59.173099999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,7 +438,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$F$12</c:f>
+              <c:f>Tabelle1!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -473,7 +473,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$13:$C$23</c:f>
+              <c:f>Tabelle1!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -515,42 +515,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$F$13:$F$23</c:f>
+              <c:f>Tabelle1!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.5446199999999999E-6</c:v>
+                  <c:v>1.5164199999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3290900000000002E-6</c:v>
+                  <c:v>1.1283099999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8669099999999999E-6</c:v>
+                  <c:v>1.1364100000000001E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5486900000000003E-6</c:v>
+                  <c:v>2.29351E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3893900000000001E-6</c:v>
+                  <c:v>3.3980899999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.23775E-5</c:v>
+                  <c:v>1.1604699999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.9958700000000005E-5</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>6.2089700000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>3.4618800000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>2.9821400000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>0.36081200000000002</c:v>
+                  <c:v>8.9463199999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7746299999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.58816E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0004699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.333011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,7 +567,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$G$12</c:f>
+              <c:f>Tabelle1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -602,7 +602,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$13:$C$23</c:f>
+              <c:f>Tabelle1!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -644,42 +644,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$G$13:$G$23</c:f>
+              <c:f>Tabelle1!$G$3:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.7376499999999999E-7</c:v>
+                  <c:v>1.89528E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4380500000000001E-7</c:v>
+                  <c:v>1.7330900000000001E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9756799999999996E-7</c:v>
+                  <c:v>6.69607E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9454200000000002E-6</c:v>
+                  <c:v>2.0471700000000001E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9764099999999998E-6</c:v>
+                  <c:v>2.8524500000000001E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4365800000000001E-6</c:v>
+                  <c:v>1.20354E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4454299999999998E-5</c:v>
+                  <c:v>5.2648899999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>3.1532700000000001E-4</c:v>
+                  <c:v>3.3755800000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>1.6437999999999999E-3</c:v>
+                  <c:v>1.7244599999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>1.1602400000000001E-2</c:v>
+                  <c:v>1.2269E-2</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>7.1822200000000003E-2</c:v>
+                  <c:v>7.81612E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,7 +745,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-AT"/>
-                  <a:t>Matrix dimensions</a:t>
+                  <a:t>Matrix dimensions (square)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -864,7 +864,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-AT"/>
-                  <a:t>runtime [s]</a:t>
+                  <a:t>time/mul [s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1579,13 +1579,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>830873</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>2198</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>678473</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>78398</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1871,275 +1871,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C12:R66"/>
+  <dimension ref="C2:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.8573699999999999E-8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.4290999999999999E-8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.5164199999999999E-6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.89528E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.40742E-8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.1853499999999999E-8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.1283099999999999E-6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.7330900000000001E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.4041000000000002E-7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.8938699999999999E-7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.1364100000000001E-6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6.69607E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.2213399999999999E-6</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.8687000000000002E-6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.29351E-6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.0471700000000001E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.8142000000000002E-6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.7430700000000001E-5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3.3980899999999999E-6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2.8524500000000001E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.7852499999999997E-5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.6868999999999998E-4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.1604699999999999E-5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.20354E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>128</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.2039E-4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.55719E-3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8.9463199999999994E-5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5.2648899999999997E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>256</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.8858499999999999E-3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.10762E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5.7746299999999996E-4</v>
+      </c>
+      <c r="G10">
+        <v>3.3755800000000001E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>512</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.5963999999999999E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.29692600000000002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.58816E-3</v>
+      </c>
+      <c r="G11">
+        <v>1.7244599999999999E-3</v>
+      </c>
+    </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1</v>
+      <c r="C12">
+        <v>1024</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.11711000000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.0330599999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3.0004699999999999E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.2269E-2</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13">
-        <v>2</v>
+        <v>2048</v>
       </c>
       <c r="D13" s="1">
-        <v>2.5166300000000001E-8</v>
+        <v>1.8560300000000001</v>
       </c>
       <c r="E13" s="1">
-        <v>2.7379200000000001E-8</v>
+        <v>59.173099999999998</v>
       </c>
       <c r="F13" s="1">
-        <v>1.5446199999999999E-6</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1.7376499999999999E-7</v>
+        <v>0.333011</v>
+      </c>
+      <c r="G13">
+        <v>7.81612E-2</v>
       </c>
       <c r="P13" s="1"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1">
-        <v>9.2736299999999994E-8</v>
-      </c>
-      <c r="E14" s="1">
-        <v>7.1905299999999997E-8</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3.3290900000000002E-6</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1.4380500000000001E-7</v>
-      </c>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3.1895199999999998E-7</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3.8974899999999998E-7</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.8669099999999999E-6</v>
-      </c>
-      <c r="G15" s="1">
-        <v>7.9756799999999996E-7</v>
-      </c>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1.15487E-6</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2.8606199999999999E-6</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4.5486900000000003E-6</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1.9454200000000002E-6</v>
-      </c>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>32</v>
-      </c>
-      <c r="D17" s="1">
-        <v>8.1165299999999997E-6</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2.7921900000000001E-5</v>
-      </c>
-      <c r="F17" s="1">
-        <v>7.3893900000000001E-6</v>
-      </c>
-      <c r="G17" s="1">
-        <v>2.9764099999999998E-6</v>
-      </c>
+    <row r="17" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.68291E-5</v>
-      </c>
-      <c r="E18">
-        <v>2.6095900000000001E-4</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1.23775E-5</v>
-      </c>
-      <c r="G18" s="1">
-        <v>8.4365800000000001E-6</v>
-      </c>
+    <row r="18" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>128</v>
-      </c>
-      <c r="D19">
-        <v>2.2247200000000001E-4</v>
-      </c>
-      <c r="E19">
-        <v>2.3298799999999999E-3</v>
-      </c>
-      <c r="F19" s="1">
-        <v>6.9958700000000005E-5</v>
-      </c>
-      <c r="G19" s="1">
-        <v>5.4454299999999998E-5</v>
-      </c>
+    <row r="19" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>256</v>
-      </c>
-      <c r="D20">
-        <v>1.5610699999999999E-3</v>
-      </c>
-      <c r="E20">
-        <v>1.9121099999999999E-2</v>
-      </c>
-      <c r="F20">
-        <v>6.2089700000000003E-4</v>
-      </c>
-      <c r="G20">
-        <v>3.1532700000000001E-4</v>
-      </c>
+    <row r="20" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>512</v>
-      </c>
-      <c r="D21">
-        <v>1.42416E-2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.25542700000000002</v>
-      </c>
-      <c r="F21">
-        <v>3.4618800000000001E-3</v>
-      </c>
-      <c r="G21">
-        <v>1.6437999999999999E-3</v>
-      </c>
+    <row r="21" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>1024</v>
-      </c>
-      <c r="D22">
-        <v>0.111112</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2.7526299999999999</v>
-      </c>
-      <c r="F22">
-        <v>2.9821400000000001E-2</v>
-      </c>
-      <c r="G22">
-        <v>1.1602400000000001E-2</v>
-      </c>
+    <row r="22" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>2048</v>
-      </c>
-      <c r="D23">
-        <v>1.66299</v>
-      </c>
-      <c r="E23" s="1">
-        <v>65.6952</v>
-      </c>
-      <c r="F23">
-        <v>0.36081200000000002</v>
-      </c>
-      <c r="G23">
-        <v>7.1822200000000003E-2</v>
-      </c>
+    <row r="23" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -2175,21 +2201,26 @@
       <c r="R39" s="1"/>
     </row>
     <row r="40" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="R41" s="1"/>
     </row>
     <row r="42" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O42" s="1"/>
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="R43" s="1"/>
     </row>
     <row r="44" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
     <row r="45" spans="15:18" x14ac:dyDescent="0.25">
@@ -2229,12 +2260,29 @@
       <c r="R52" s="1"/>
     </row>
     <row r="53" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="R53" s="1"/>
     </row>
     <row r="54" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="R54" s="1"/>
+    </row>
+    <row r="55" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O59" s="1"/>
     </row>
     <row r="60" spans="15:18" x14ac:dyDescent="0.25">
       <c r="P60" s="1"/>

</xml_diff>